<commit_message>
code und personal änderung
</commit_message>
<xml_diff>
--- a/data/cleaned_data/Personal.xlsx
+++ b/data/cleaned_data/Personal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\uni\DALI\excel datein\richtig\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathan.bach/Documents/GitHub/Repositorys/Streamlit-Application-for-Data-Literacy-1/data/cleaned_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB79CBD4-7E5C-4984-B881-019002520079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62503209-F5B9-2048-A44E-E27658567D90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4910" yWindow="90" windowWidth="14400" windowHeight="7270" xr2:uid="{77372379-03CE-484A-878A-6D1123912F0D}"/>
+    <workbookView xWindow="4920" yWindow="740" windowWidth="14400" windowHeight="7280" xr2:uid="{77372379-03CE-484A-878A-6D1123912F0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -51,46 +51,46 @@
     <t>Nichtärztliches Personal im Pflegedienst</t>
   </si>
   <si>
-    <t>31.12.2010</t>
-  </si>
-  <si>
-    <t>31.12.2011</t>
-  </si>
-  <si>
-    <t>31.12.2012</t>
-  </si>
-  <si>
-    <t>31.12.2013</t>
-  </si>
-  <si>
-    <t>31.12.2014</t>
-  </si>
-  <si>
-    <t>31.12.2015</t>
-  </si>
-  <si>
-    <t>31.12.2016</t>
-  </si>
-  <si>
-    <t>31.12.2017</t>
-  </si>
-  <si>
-    <t>31.12.2018</t>
-  </si>
-  <si>
-    <t>31.12.2019</t>
-  </si>
-  <si>
-    <t>31.12.2020</t>
-  </si>
-  <si>
-    <t>31.12.2021</t>
-  </si>
-  <si>
-    <t>31.12.2022</t>
-  </si>
-  <si>
-    <t>31.12.2023</t>
+    <t>2010</t>
+  </si>
+  <si>
+    <t>2011</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>2012</t>
+  </si>
+  <si>
+    <t>2013</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>2023</t>
   </si>
 </sst>
 </file>
@@ -108,6 +108,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -135,7 +136,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -170,9 +171,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -210,7 +211,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -316,7 +317,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -458,7 +459,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -468,13 +469,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{971D4CCF-CCBD-4C90-9A3E-0B1E7DF51D76}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -491,7 +492,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -508,7 +509,7 @@
         <v>406269</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -525,9 +526,9 @@
         <v>411920</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1">
         <v>1154411</v>
@@ -542,9 +543,9 @@
         <v>414884</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1">
         <v>1172077</v>
@@ -559,9 +560,9 @@
         <v>419140</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1">
         <v>1186650</v>
@@ -576,9 +577,9 @@
         <v>422779</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1">
         <v>1200849</v>
@@ -593,9 +594,9 @@
         <v>426838</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1">
         <v>1223859</v>
@@ -610,9 +611,9 @@
         <v>433434</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1">
         <v>1246121</v>
@@ -627,9 +628,9 @@
         <v>437648</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1">
         <v>1259838</v>
@@ -644,9 +645,9 @@
         <v>437799</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1">
         <v>1305430</v>
@@ -661,9 +662,9 @@
         <v>457947</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1">
         <v>1347524</v>
@@ -678,9 +679,9 @@
         <v>486085</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B13" s="1">
         <v>1369562</v>
@@ -695,7 +696,7 @@
         <v>497529</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
@@ -712,7 +713,7 @@
         <v>509104</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>

</xml_diff>